<commit_message>
comments based on new results
</commit_message>
<xml_diff>
--- a/tcc_android_pattern/ckjm-1.9/metrics/analise_dados.xlsx
+++ b/tcc_android_pattern/ckjm-1.9/metrics/analise_dados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="5" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="271" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="6" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="271" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,13 +14,14 @@
     <sheet name="package_group_iteracao_1" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="package_group_baseline_2" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="package_group_list_detail_2" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="package_group_list_editor" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="466">
   <si>
     <t>WMC</t>
   </si>
@@ -1415,6 +1416,9 @@
   </si>
   <si>
     <t>SEM ANONYMOUS INNER CLASSES</t>
+  </si>
+  <si>
+    <t>com.android.contacts.group.GroupEditorPresenter$GroupEditorMemento</t>
   </si>
 </sst>
 </file>
@@ -30630,7 +30634,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
-      <selection activeCell="K12" activeCellId="0" pane="topLeft" sqref="K12"/>
+      <selection activeCell="H17" activeCellId="0" pane="topLeft" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -31453,10 +31457,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
-      <selection activeCell="H29" activeCellId="0" pane="topLeft" sqref="H29"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
+      <selection activeCell="A28" activeCellId="0" pane="topLeft" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -31465,7 +31469,7 @@
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -31525,7 +31529,7 @@
       </c>
       <c r="N2" s="6" t="n">
         <f aca="false">AVERAGE(B2:B34)</f>
-        <v>11.95</v>
+        <v>12.4736842105263</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
@@ -31552,7 +31556,7 @@
       </c>
       <c r="N3" s="5" t="n">
         <f aca="false">AVERAGE(C2:C34)</f>
-        <v>0.65</v>
+        <v>0.631578947368421</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
@@ -31602,11 +31606,11 @@
       </c>
       <c r="M5" s="2" t="n">
         <f aca="false">MAX(E2:E449)</f>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N5" s="6" t="n">
         <f aca="false">AVERAGE(E2:E34)</f>
-        <v>11.55</v>
+        <v>12.1052631578947</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="6">
@@ -31614,7 +31618,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>0</v>
@@ -31626,16 +31630,16 @@
         <v>36</v>
       </c>
       <c r="F6" s="6" t="n">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G6" s="6" t="n">
-        <v>466</v>
+        <v>456</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>8</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2" t="s">
@@ -31647,11 +31651,11 @@
       </c>
       <c r="M6" s="2" t="n">
         <f aca="false">MAX(F2:F449)</f>
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N6" s="6" t="n">
         <f aca="false">AVERAGE(F2:F34)</f>
-        <v>33.35</v>
+        <v>34.8421052631579</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="7">
@@ -31696,10 +31700,10 @@
       </c>
       <c r="N7" s="6" t="n">
         <f aca="false">AVERAGE(G2:G34)</f>
-        <v>82.85</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+        <v>86.6842105263158</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="8">
       <c r="A8" s="2" t="s">
         <v>260</v>
       </c>
@@ -31729,7 +31733,7 @@
       </c>
       <c r="J8" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="9">
       <c r="A9" s="2" t="s">
         <v>111</v>
       </c>
@@ -31801,7 +31805,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="13">
       <c r="A13" s="2" t="s">
         <v>155</v>
       </c>
@@ -31831,7 +31835,7 @@
       </c>
       <c r="J13" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="14">
       <c r="A14" s="2" t="s">
         <v>222</v>
       </c>
@@ -31861,7 +31865,7 @@
       </c>
       <c r="J14" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="15">
       <c r="A15" s="2" t="s">
         <v>316</v>
       </c>
@@ -31891,7 +31895,7 @@
       </c>
       <c r="J15" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="16">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -31905,10 +31909,10 @@
         <v>0</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>772</v>
@@ -31921,7 +31925,7 @@
       </c>
       <c r="J16" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="17">
       <c r="A17" s="2" t="s">
         <v>118</v>
       </c>
@@ -31951,7 +31955,7 @@
       </c>
       <c r="J17" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="18">
       <c r="A18" s="2" t="s">
         <v>191</v>
       </c>
@@ -32011,7 +32015,7 @@
       </c>
       <c r="J19" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
         <v>97</v>
       </c>
@@ -32089,7 +32093,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="25">
       <c r="A25" s="2" t="s">
         <v>194</v>
       </c>
@@ -32119,12 +32123,12 @@
       </c>
       <c r="J25" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="26">
       <c r="A26" s="2" t="s">
-        <v>461</v>
+        <v>77</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>1</v>
@@ -32133,46 +32137,46 @@
         <v>0</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I26" s="2" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J26" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="27">
       <c r="A27" s="2" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>31</v>
+        <v>119</v>
       </c>
       <c r="H27" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I27" s="2" t="n">
         <v>10</v>
@@ -32180,53 +32184,53 @@
       <c r="J27" s="2"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
-      <c r="A28" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="C28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" s="2" t="n">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="29">
+      <c r="A29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="F28" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="G28" s="2" t="n">
-        <v>119</v>
-      </c>
-      <c r="H28" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="I28" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="J28" s="2"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
+      <c r="C29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I29" s="2" t="n">
+        <v>11</v>
+      </c>
       <c r="J29" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="30">
       <c r="A30" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>0</v>
@@ -32235,16 +32239,16 @@
         <v>0</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I30" s="2" t="n">
         <v>11</v>
@@ -32253,106 +32257,77 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="31">
       <c r="A31" s="2" t="s">
-        <v>37</v>
+        <v>88</v>
       </c>
       <c r="B31" s="6" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E31" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="F31" s="6" t="n">
         <v>27</v>
       </c>
-      <c r="F31" s="6" t="n">
-        <v>64</v>
-      </c>
       <c r="G31" s="6" t="n">
-        <v>83</v>
+        <v>24</v>
       </c>
       <c r="H31" s="2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I31" s="2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J31" s="2"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
-      <c r="A32" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B32" s="2" t="n">
-        <v>13</v>
-      </c>
-      <c r="C32" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D32" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E32" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="F32" s="2" t="n">
-        <v>27</v>
-      </c>
-      <c r="G32" s="2" t="n">
-        <v>24</v>
-      </c>
-      <c r="H32" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="I32" s="2" t="n">
-        <v>10</v>
-      </c>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="33">
+      <c r="A33" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="B33" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="F33" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="G33" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="H33" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I33" s="2" t="n">
+        <v>9</v>
+      </c>
       <c r="J33" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="34">
-      <c r="A34" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="B34" s="2" t="n">
-        <v>14</v>
-      </c>
-      <c r="C34" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D34" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E34" s="2" t="n">
-        <v>14</v>
-      </c>
-      <c r="F34" s="2" t="n">
-        <v>33</v>
-      </c>
-      <c r="G34" s="2" t="n">
-        <v>21</v>
-      </c>
-      <c r="H34" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I34" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="J34" s="2"/>
-    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37"/>
@@ -32379,395 +32354,930 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="60"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="62"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="63"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="64"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="65"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="66"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="67"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="68"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="69"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="70"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="71"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="72"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="73"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="74"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="75"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="76"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="77"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="78"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="79"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="80"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="81"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="82"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="83"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="84"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="85"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="86"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="87"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="88"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="89"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="90"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="91"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="92"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="93"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="94"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="95"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="96"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="97"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="98"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="99"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="100"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="101"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="102"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="103"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="104"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="105"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="106"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="107"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="108"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="109"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="110"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="111"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="112"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="113"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="114"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="115"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="116"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="117"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="118"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="119"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="120"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="121"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="122"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="123"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="124"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="125"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="126"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="127"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="128"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="129"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="130"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="131"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="132"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="133"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="134"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="135"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="136"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="137"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="138"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="139"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="140"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="141"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="142"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="143"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="144"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="145"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="146"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="147"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="148"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="149"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="150"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="151"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="152"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="153"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="154"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="155"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="156"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="157"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="158"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="159"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="160"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="161"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="162"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="163"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="164"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="165"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="166"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="167"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="168"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="169"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="170"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="171"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="172"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="173"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="174"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="175"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="176"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="177"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="178"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="179"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="180"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="181"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="182"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="183"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="184"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="185"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="186"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="187"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="188"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="189"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="190"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="191"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="192"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="193"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="194"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="195"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="196"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="197"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="198"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="199"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="200"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="201"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="202"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="203"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="204"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="205"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="206"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="207"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="208"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="209"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="210"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="211"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="212"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="213"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="214"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="215"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="216"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="217"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="218"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="219"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="220"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="221"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="222"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="223"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="224"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="225"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="226"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="227"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="228"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="229"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="230"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="231"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="232"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="233"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="234"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="235"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="236"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="237"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="238"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="239"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="240"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="241"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="242"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="243"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="244"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="245"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="246"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="247"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="248"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="249"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="250"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="251"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="252"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="253"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="254"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="255"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="256"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="257"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="258"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="259"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="260"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="261"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="262"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="263"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="264"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="265"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="266"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="267"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="268"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="269"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="270"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="271"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="272"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="273"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="274"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="275"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="276"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="277"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="278"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="279"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="280"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="281"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="282"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="283"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="284"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="285"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="286"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="287"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="288"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="289"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="290"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="291"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="292"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="293"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="294"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="295"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="296"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="297"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="298"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="299"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="300"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="301"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="302"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="303"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="304"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="305"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="306"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="307"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="308"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="309"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="310"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="311"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="312"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="313"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="314"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="315"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="316"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="317"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="318"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="319"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="320"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="321"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="322"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="323"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="324"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="325"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="326"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="327"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="328"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="329"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="330"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="331"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="332"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="333"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="334"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="335"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="336"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="337"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="338"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="339"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="340"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="341"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="342"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="343"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="344"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="345"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="346"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="347"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="348"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="349"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="350"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="351"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="352"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="353"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="354"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="355"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="356"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="357"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="358"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="359"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="360"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="361"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="362"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="363"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="364"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="365"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="366"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="367"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="368"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="369"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="370"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="371"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="372"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="373"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="374"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="375"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="376"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="377"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="378"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="379"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="380"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="381"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="382"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="383"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="384"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="385"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="386"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="387"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="388"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="389"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="390"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="391"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="392"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="393"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="394"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="395"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="396"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="397"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="398"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="399"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="400"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="401"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="402"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="403"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="404"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="405"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="406"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="407"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="408"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="409"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="410"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="411"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="412"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="413"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="414"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="415"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="416"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="417"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="418"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="419"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="420"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="421"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="422"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="423"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="424"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="425"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="426"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="427"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="428"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="429"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="430"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="431"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="432"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="433"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="434"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="435"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="436"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="437"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="438"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="439"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="440"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="441"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="442"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="443"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="444"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="445"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="446"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="447"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="448"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="449"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N34"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="72.1581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="L1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <f aca="false">MIN(B2:B449)</f>
+        <v>1</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <f aca="false">MAX(B2:B449)</f>
+        <v>45</v>
+      </c>
+      <c r="N2" s="6" t="n">
+        <f aca="false">AVERAGE(B2:B34)</f>
+        <v>11.9047619047619</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <f aca="false">MIN(C2:C449)</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <f aca="false">MAX(C2:C449)</f>
+        <v>2</v>
+      </c>
+      <c r="N3" s="5" t="n">
+        <f aca="false">AVERAGE(C2:C34)</f>
+        <v>0.666666666666667</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>456</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="2" t="n">
+        <f aca="false">MIN(C2:C449)</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="2" t="n">
+        <f aca="false">MAX(D2:D449)</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="2" t="n">
+        <f aca="false">AVERAGE(D2:D34)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+      <c r="A5" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <f aca="false">MIN(E2:E449)</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="2" t="n">
+        <f aca="false">MAX(E2:E449)</f>
+        <v>46</v>
+      </c>
+      <c r="N5" s="6" t="n">
+        <f aca="false">AVERAGE(E2:E34)</f>
+        <v>11.8571428571429</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+      <c r="A6" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <f aca="false">MIN(F2:F449)</f>
+        <v>1</v>
+      </c>
+      <c r="M6" s="2" t="n">
+        <f aca="false">MAX(F2:F449)</f>
+        <v>141</v>
+      </c>
+      <c r="N6" s="6" t="n">
+        <f aca="false">AVERAGE(F2:F34)</f>
+        <v>33.5714285714286</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+      <c r="A7" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L7" s="2" t="n">
+        <f aca="false">MIN(G2:G449)</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="2" t="n">
+        <f aca="false">MAX(G2:G449)</f>
+        <v>646</v>
+      </c>
+      <c r="N7" s="6" t="n">
+        <f aca="false">AVERAGE(G2:G34)</f>
+        <v>73.9047619047619</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="3" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="3" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+      <c r="A12" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="J12" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+      <c r="A13" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="J13" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+      <c r="A14" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>141</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>646</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="J15" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+      <c r="A16" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J16" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+      <c r="A17" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="J17" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+      <c r="A18" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="I18" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="J18" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+      <c r="A19" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="J19" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+      <c r="J20" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+      <c r="A24" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="F24" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="G24" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I24" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="J24" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
+      <c r="A25" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="G25" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I25" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="J25" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+      <c r="A26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="G26" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I26" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="J26" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
+      <c r="A27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>119</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="I27" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="J27" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+      <c r="A29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I29" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="J29" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+      <c r="A30" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
+      <c r="A31" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="6" t="n">
+        <v>22</v>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="6" t="n">
+        <v>27</v>
+      </c>
+      <c r="F31" s="6" t="n">
+        <v>64</v>
+      </c>
+      <c r="G31" s="6" t="n">
+        <v>83</v>
+      </c>
+      <c r="H31" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="I31" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="J31" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
+      <c r="A32" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="G32" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="H32" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="I32" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="J32" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
+      <c r="A34" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
generate Graphics and explain execution
</commit_message>
<xml_diff>
--- a/tcc_android_pattern/ckjm-1.9/metrics/analise_dados.xlsx
+++ b/tcc_android_pattern/ckjm-1.9/metrics/analise_dados.xlsx
@@ -5,21 +5,21 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="271" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="4" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="271" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Iteração 1" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Iteração 2" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Iteração 3" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Iteração1" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Iteração2" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Iteração3" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="graficos" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="53">
   <si>
     <t>WMC</t>
   </si>
@@ -147,6 +147,9 @@
     <t>com.android.contacts.group.GroupEditorFragment$CancelEditDialogFragment$1</t>
   </si>
   <si>
+    <t>DIFF</t>
+  </si>
+  <si>
     <t>com.android.contacts.group.GroupDetailPresenter</t>
   </si>
   <si>
@@ -161,6 +164,21 @@
   <si>
     <t>com.android.contacts.group.GroupEditorPresenter$GroupEditorMemento</t>
   </si>
+  <si>
+    <t>CATEGORIAS</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>Iteração 1</t>
+  </si>
+  <si>
+    <t>Iteração 2</t>
+  </si>
+  <si>
+    <t>Iteração 3</t>
+  </si>
 </sst>
 </file>
 
@@ -169,12 +187,11 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -195,7 +212,11 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -262,7 +283,2272 @@
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF7E0021"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF83CAFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFD320"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF420E"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF004586"/>
+      <rgbColor rgb="FF579D1C"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>wmc</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>wmc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>graficos!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Iteração 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Iteração 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Iteração 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>baseline!$N$2,Iteração1!$N$2,Iteração2!$N$2,Iteração3!$N$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.51612903225806</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.93939393939394</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="92086319"/>
+        <c:axId val="12710659"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="92086319"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr sz="900"/>
+                  <a:t>Iterações</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="12710659"/>
+        <c:crossesAt val="0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="12710659"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="92086319"/>
+        <c:crossesAt val="0"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>dit</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>dit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>graficos!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Iteração 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Iteração 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Iteração 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>baseline!$N$3,Iteração1!$N$3,Iteração2!$N$3,Iteração3!$N$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.774193548387097</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.78125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.787878787878788</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="1682800"/>
+        <c:axId val="25218124"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1682800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="25218124"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="25218124"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="1682800"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>noc</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>noc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>graficos!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Iteração 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Iteração 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Iteração 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>baseline!$N$4,Iteração1!$N$4,Iteração2!$N$4,Iteração3!$N$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="47830757"/>
+        <c:axId val="89986599"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="47830757"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="89986599"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="89986599"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="47830757"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>cbo</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cbo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>graficos!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Iteração 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Iteração 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Iteração 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>baseline!$N$5,Iteração1!$N$5,Iteração2!$N$5,Iteração3!$N$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10.1612903225806</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.03125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.09375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.1515151515152</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="73132128"/>
+        <c:axId val="51423322"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="73132128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="51423322"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="51423322"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="73132128"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>rfc</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rfc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>graficos!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Iteração 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Iteração 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Iteração 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>baseline!$N$6,Iteração1!$N$6,Iteração2!$N$6,Iteração3!$N$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>23.741935483871</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.21875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.71875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.9090909090909</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="84581258"/>
+        <c:axId val="82273276"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="84581258"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="82273276"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="82273276"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="84581258"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lcom</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>lcom</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>graficos!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Iteração 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Iteração 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Iteração 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>baseline!$N$7,Iteração1!$N$7,Iteração2!$N$7,Iteração3!$N$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>57.4838709677419</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>56.875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.1875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48.4242424242424</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="73067927"/>
+        <c:axId val="83841422"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="73067927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="83841422"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="83841422"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="73067927"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>wmc</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>wmc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>graficos!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Iteração 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Iteração 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>baseline!$N$2,Iteração1!$N$2,Iteração2!$N$2,Iteração3!$N$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.51612903225806</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.93939393939394</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>dit</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>dit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>graficos!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Iteração 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Iteração 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>baseline!$N$3,Iteração1!$N$3,Iteração2!$N$3,Iteração3!$N$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.774193548387097</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.78125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.787878787878788</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>noc</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>noc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>graficos!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Iteração 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Iteração 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>$baseline.$n$4$iteração1.$n$4,Iteração2!$N$4,Iteração3!$N$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>cbo</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cbo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="579d1c"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>graficos!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Iteração 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Iteração 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>baseline!$N$5,Iteração1!$N$5,Iteração2!$N$5,Iteração3!$N$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10.1612903225806</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.03125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.09375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.1515151515152</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>rfc</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rfc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7e0021"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>graficos!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Iteração 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Iteração 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>baseline!$N$6,Iteração1!$N$6,Iteração2!$N$6,Iteração3!$N$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>23.741935483871</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.21875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.71875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.9090909090909</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lcom</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>lcom</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="83caff"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>graficos!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Iteração 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Iteração 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>baseline!$N$7,Iteração1!$N$7,Iteração2!$N$7,Iteração3!$N$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>57.4838709677419</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>56.875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.1875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48.4242424242424</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="2410365"/>
+        <c:axId val="22979052"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2410365"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="22979052"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="22979052"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="2410365"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>16200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>693720</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>154440</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="1641600" y="0"/>
+        <a:ext cx="5554440" cy="3499920"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>155520</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>70560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>225720</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>118080</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="7470720" y="223920"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>773280</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>124920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>29520</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>5400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="1585800" y="3786840"/>
+        <a:ext cx="5758920" cy="3232080"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>125280</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>100440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>195480</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>151200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="7440480" y="3762360"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>799560</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>138600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>56520</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>144720</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="1612080" y="7314480"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>36360</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>71640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>106560</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>77760</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="7351560" y="7247520"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>545400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>29520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>614880</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>77400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="13550040" y="497160"/>
+        <a:ext cx="5758920" cy="3242160"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -270,15 +2556,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C52" activeCellId="0" pane="topLeft" sqref="C52"/>
+      <selection activeCell="A52" activeCellId="0" pane="topLeft" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="72.1581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -316,7 +2603,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>11</v>
       </c>
@@ -360,7 +2647,7 @@
         <v>8.51612903225806</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>12</v>
       </c>
@@ -404,7 +2691,7 @@
         <v>0.774193548387097</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
         <v>13</v>
       </c>
@@ -448,7 +2735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
         <v>14</v>
       </c>
@@ -638,7 +2925,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
         <v>19</v>
       </c>
@@ -667,7 +2954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
         <v>20</v>
       </c>
@@ -696,7 +2983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
         <v>21</v>
       </c>
@@ -725,7 +3012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
         <v>22</v>
       </c>
@@ -957,7 +3244,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
         <v>30</v>
       </c>
@@ -986,7 +3273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
         <v>31</v>
       </c>
@@ -1015,7 +3302,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
         <v>32</v>
       </c>
@@ -1044,7 +3331,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
         <v>33</v>
       </c>
@@ -1160,7 +3447,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
         <v>37</v>
       </c>
@@ -1276,7 +3563,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
         <v>41</v>
       </c>
@@ -1305,13 +3592,14 @@
         <v>1</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1324,7 +3612,7 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="N2" activeCellId="0" pane="topLeft" sqref="N2"/>
+      <selection activeCell="N10" activeCellId="0" pane="topLeft" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1368,7 +3656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>11</v>
       </c>
@@ -1412,7 +3700,7 @@
         <v>8.875</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>12</v>
       </c>
@@ -1456,7 +3744,7 @@
         <v>0.78125</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
         <v>13</v>
       </c>
@@ -1500,7 +3788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
         <v>14</v>
       </c>
@@ -1690,7 +3978,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
         <v>19</v>
       </c>
@@ -1718,8 +4006,11 @@
       <c r="I10" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+      <c r="N10" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
         <v>20</v>
       </c>
@@ -1747,8 +4038,12 @@
       <c r="I11" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+      <c r="N11" s="0" t="n">
+        <f aca="false">N2-baseline!$N$2</f>
+        <v>0.358870967741936</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
         <v>21</v>
       </c>
@@ -1776,8 +4071,12 @@
       <c r="I12" s="0" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+      <c r="N12" s="0" t="n">
+        <f aca="false">N3-baseline!$N$3</f>
+        <v>0.00705645161290325</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
         <v>22</v>
       </c>
@@ -1805,8 +4104,12 @@
       <c r="I13" s="0" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+      <c r="N13" s="0" t="n">
+        <f aca="false">N4-baseline!$N$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
         <v>23</v>
       </c>
@@ -1834,8 +4137,12 @@
       <c r="I14" s="0" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+      <c r="N14" s="0" t="n">
+        <f aca="false">N5-baseline!$N$5</f>
+        <v>-0.130040322580646</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
         <v>24</v>
       </c>
@@ -1863,8 +4170,12 @@
       <c r="I15" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+      <c r="N15" s="0" t="n">
+        <f aca="false">N6-baseline!$N$6</f>
+        <v>0.476814516129032</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
         <v>25</v>
       </c>
@@ -1892,8 +4203,12 @@
       <c r="I16" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+      <c r="N16" s="0" t="n">
+        <f aca="false">N7-baseline!$N$7</f>
+        <v>-0.608870967741936</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
         <v>26</v>
       </c>
@@ -1922,7 +4237,7 @@
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
         <v>27</v>
       </c>
@@ -1951,7 +4266,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
         <v>28</v>
       </c>
@@ -1980,9 +4295,9 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>19</v>
@@ -2009,7 +4324,7 @@
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
         <v>29</v>
       </c>
@@ -2038,7 +4353,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
         <v>30</v>
       </c>
@@ -2067,7 +4382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
         <v>31</v>
       </c>
@@ -2096,7 +4411,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
         <v>32</v>
       </c>
@@ -2125,7 +4440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
         <v>33</v>
       </c>
@@ -2241,7 +4556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
         <v>37</v>
       </c>
@@ -2328,7 +4643,7 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
         <v>40</v>
       </c>
@@ -2388,11 +4703,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2404,13 +4719,14 @@
   </sheetPr>
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="N2" activeCellId="0" pane="topLeft" sqref="N2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A44" activeCellId="0" pane="topLeft" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="72.1581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -2448,7 +4764,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>11</v>
       </c>
@@ -2492,7 +4808,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>12</v>
       </c>
@@ -2536,7 +4852,7 @@
         <v>0.78125</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
         <v>13</v>
       </c>
@@ -2580,7 +4896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
         <v>14</v>
       </c>
@@ -2624,7 +4940,7 @@
         <v>10.09375</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
         <v>15</v>
       </c>
@@ -2668,7 +4984,7 @@
         <v>24.71875</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
         <v>16</v>
       </c>
@@ -2712,7 +5028,7 @@
         <v>53.1875</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
         <v>17</v>
       </c>
@@ -2741,7 +5057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
         <v>18</v>
       </c>
@@ -2770,7 +5086,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
         <v>19</v>
       </c>
@@ -2798,8 +5114,11 @@
       <c r="I10" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+      <c r="N10" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
         <v>20</v>
       </c>
@@ -2827,8 +5146,12 @@
       <c r="I11" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+      <c r="N11" s="0" t="n">
+        <f aca="false">N2-Iteração1!$N$2</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
         <v>22</v>
       </c>
@@ -2856,8 +5179,12 @@
       <c r="I12" s="0" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+      <c r="N12" s="0" t="n">
+        <f aca="false">N3-Iteração1!$N$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
         <v>23</v>
       </c>
@@ -2885,8 +5212,12 @@
       <c r="I13" s="0" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+      <c r="N13" s="0" t="n">
+        <f aca="false">N4-Iteração1!$N$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
         <v>24</v>
       </c>
@@ -2914,8 +5245,12 @@
       <c r="I14" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+      <c r="N14" s="0" t="n">
+        <f aca="false">N5-Iteração1!$N$5</f>
+        <v>0.0625</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
         <v>25</v>
       </c>
@@ -2943,8 +5278,12 @@
       <c r="I15" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+      <c r="N15" s="0" t="n">
+        <f aca="false">N6-Iteração1!$N$6</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
         <v>26</v>
       </c>
@@ -2971,6 +5310,10 @@
       </c>
       <c r="I16" s="0" t="n">
         <v>16</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <f aca="false">N7-Iteração1!$N$7</f>
+        <v>-3.6875</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
@@ -3033,7 +5376,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>19</v>
@@ -3089,7 +5432,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
         <v>30</v>
       </c>
@@ -3118,7 +5461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
         <v>31</v>
       </c>
@@ -3147,7 +5490,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
         <v>32</v>
       </c>
@@ -3176,7 +5519,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
         <v>33</v>
       </c>
@@ -3292,7 +5635,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
         <v>37</v>
       </c>
@@ -3439,7 +5782,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>14</v>
@@ -3468,11 +5811,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -3485,12 +5828,13 @@
   <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D52" activeCellId="0" pane="topLeft" sqref="D52"/>
+      <selection activeCell="N16" activeCellId="0" pane="topLeft" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="86.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -3528,7 +5872,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>11</v>
       </c>
@@ -3568,11 +5912,11 @@
         <v>45</v>
       </c>
       <c r="N2" s="2" t="n">
-        <f aca="false">AVERAGE(B2:B449)</f>
+        <f aca="false">AVERAGE(B2:B34)</f>
         <v>8.93939393939394</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>13</v>
       </c>
@@ -3612,7 +5956,7 @@
         <v>2</v>
       </c>
       <c r="N3" s="2" t="n">
-        <f aca="false">AVERAGE(C2:C449)</f>
+        <f aca="false">AVERAGE(C2:C34)</f>
         <v>0.787878787878788</v>
       </c>
     </row>
@@ -3656,7 +6000,7 @@
         <v>0</v>
       </c>
       <c r="N4" s="2" t="n">
-        <f aca="false">AVERAGE(D2:D449)</f>
+        <f aca="false">AVERAGE(D2:D34)</f>
         <v>0</v>
       </c>
     </row>
@@ -3700,7 +6044,7 @@
         <v>46</v>
       </c>
       <c r="N5" s="2" t="n">
-        <f aca="false">AVERAGE(E2:E449)</f>
+        <f aca="false">AVERAGE(E2:E34)</f>
         <v>10.1515151515152</v>
       </c>
     </row>
@@ -3744,7 +6088,7 @@
         <v>141</v>
       </c>
       <c r="N6" s="2" t="n">
-        <f aca="false">AVERAGE(F2:F449)</f>
+        <f aca="false">AVERAGE(F2:F34)</f>
         <v>24.9090909090909</v>
       </c>
     </row>
@@ -3788,13 +6132,13 @@
         <v>646</v>
       </c>
       <c r="N7" s="2" t="n">
-        <f aca="false">AVERAGE(G2:G449)</f>
+        <f aca="false">AVERAGE(G2:G34)</f>
         <v>48.4242424242424</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>6</v>
@@ -3850,7 +6194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
         <v>20</v>
       </c>
@@ -3878,8 +6222,11 @@
       <c r="I10" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+      <c r="N10" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
         <v>22</v>
       </c>
@@ -3907,8 +6254,12 @@
       <c r="I11" s="0" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+      <c r="N11" s="0" t="n">
+        <f aca="false">N2-Iteração2!$N$2</f>
+        <v>-0.0606060606060606</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
         <v>23</v>
       </c>
@@ -3936,8 +6287,12 @@
       <c r="I12" s="0" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+      <c r="N12" s="0" t="n">
+        <f aca="false">N3-Iteração2!$N$3</f>
+        <v>0.00662878787878785</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
         <v>24</v>
       </c>
@@ -3965,8 +6320,12 @@
       <c r="I13" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+      <c r="N13" s="0" t="n">
+        <f aca="false">N4-Iteração2!$N$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
         <v>25</v>
       </c>
@@ -3994,8 +6353,12 @@
       <c r="I14" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+      <c r="N14" s="0" t="n">
+        <f aca="false">N5-Iteração2!$N$5</f>
+        <v>0.0577651515151523</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
         <v>26</v>
       </c>
@@ -4023,8 +6386,12 @@
       <c r="I15" s="0" t="n">
         <v>19</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+      <c r="N15" s="0" t="n">
+        <f aca="false">N6-Iteração2!$N$6</f>
+        <v>0.19034090909091</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
         <v>27</v>
       </c>
@@ -4051,6 +6418,10 @@
       </c>
       <c r="I16" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <f aca="false">N7-Iteração2!$N$7</f>
+        <v>-4.76325757575758</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
@@ -4084,7 +6455,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>19</v>
@@ -4140,7 +6511,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
         <v>30</v>
       </c>
@@ -4169,7 +6540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
         <v>31</v>
       </c>
@@ -4198,7 +6569,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
         <v>32</v>
       </c>
@@ -4227,7 +6598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
         <v>33</v>
       </c>
@@ -4287,7 +6658,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>15</v>
@@ -4372,7 +6743,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
         <v>37</v>
       </c>
@@ -4432,7 +6803,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1</v>
@@ -4517,7 +6888,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
         <v>41</v>
       </c>
@@ -4548,7 +6919,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>14</v>
@@ -4577,11 +6948,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4591,10 +6962,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="F1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="V31" activeCellId="0" pane="topLeft" sqref="V31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4602,14 +6973,54 @@
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
+      <c r="A4" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="51"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
revisão resultados da pesquisa e resultados
</commit_message>
<xml_diff>
--- a/tcc_android_pattern/ckjm-1.9/metrics/analise_dados.xlsx
+++ b/tcc_android_pattern/ckjm-1.9/metrics/analise_dados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="3" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="271" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="4" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="271" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="1" state="visible" r:id="rId2"/>
@@ -412,7 +412,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="6"/>
+            <c:size val="5"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -483,27 +483,27 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.774193548387097</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.78125</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.78125</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.787878787878788</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="68401784"/>
-        <c:axId val="51531525"/>
+        <c:axId val="22213466"/>
+        <c:axId val="41284721"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68401784"/>
+        <c:axId val="22213466"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -519,14 +519,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="51531525"/>
+        <c:crossAx val="41284721"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51531525"/>
+        <c:axId val="41284721"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -551,7 +551,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="68401784"/>
+        <c:crossAx val="22213466"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -638,7 +638,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="6"/>
+            <c:size val="5"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -709,27 +709,27 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="588414"/>
-        <c:axId val="13274166"/>
+        <c:axId val="24168142"/>
+        <c:axId val="81898758"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="588414"/>
+        <c:axId val="24168142"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -745,14 +745,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="13274166"/>
+        <c:crossAx val="81898758"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="13274166"/>
+        <c:axId val="81898758"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -777,7 +777,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="588414"/>
+        <c:crossAx val="24168142"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -864,7 +864,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="6"/>
+            <c:size val="5"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -935,27 +935,27 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.1612903225806</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.03125</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.09375</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.1515151515152</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="12582092"/>
-        <c:axId val="38618866"/>
+        <c:axId val="61533663"/>
+        <c:axId val="10940117"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="12582092"/>
+        <c:axId val="61533663"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -971,14 +971,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="38618866"/>
+        <c:crossAx val="10940117"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38618866"/>
+        <c:axId val="10940117"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1003,7 +1003,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="12582092"/>
+        <c:crossAx val="61533663"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1090,7 +1090,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="6"/>
+            <c:size val="5"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -1161,27 +1161,27 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>23.741935483871</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.21875</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.71875</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.9090909090909</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="45471841"/>
-        <c:axId val="42216467"/>
+        <c:axId val="16874101"/>
+        <c:axId val="20449600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45471841"/>
+        <c:axId val="16874101"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1197,14 +1197,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="42216467"/>
+        <c:crossAx val="20449600"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42216467"/>
+        <c:axId val="20449600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1229,7 +1229,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="45471841"/>
+        <c:crossAx val="16874101"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1316,7 +1316,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="6"/>
+            <c:size val="5"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -1387,27 +1387,27 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>57.4838709677419</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>56.875</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53.1875</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>48.4242424242424</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="65804461"/>
-        <c:axId val="15543459"/>
+        <c:axId val="68952474"/>
+        <c:axId val="80088686"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="65804461"/>
+        <c:axId val="68952474"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1423,14 +1423,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="15543459"/>
+        <c:crossAx val="80088686"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15543459"/>
+        <c:axId val="80088686"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1455,7 +1455,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="65804461"/>
+        <c:crossAx val="68952474"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1524,7 +1524,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="6"/>
+            <c:size val="5"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -1633,7 +1633,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="6"/>
+            <c:size val="5"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -1742,7 +1742,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="6"/>
+            <c:size val="5"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -1765,6 +1765,26 @@
               <c:showPercent val="0"/>
               <c:separator> </c:separator>
             </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator>; </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator>; </c:separator>
+            </c:dLbl>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1785,14 +1805,20 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>$baseline.$n$4$iteração1.$n$4,Iteração2!$N$4,Iteração3!$N$4</c:f>
+              <c:f>baseline!$N$4,Iteração1!$N$4,Iteração2!$N$4,Iteração3!$N$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1825,7 +1851,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="6"/>
+            <c:size val="5"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -1934,7 +1960,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="6"/>
+            <c:size val="5"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -2043,7 +2069,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="6"/>
+            <c:size val="5"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -2127,11 +2153,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="13739932"/>
-        <c:axId val="37263911"/>
+        <c:axId val="54379820"/>
+        <c:axId val="52702933"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="13739932"/>
+        <c:axId val="54379820"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2147,14 +2173,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="37263911"/>
+        <c:crossAx val="52702933"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37263911"/>
+        <c:axId val="52702933"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2179,7 +2205,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="13739932"/>
+        <c:crossAx val="54379820"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2266,7 +2292,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="6"/>
+            <c:size val="5"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -2337,27 +2363,27 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8.51612903225806</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.875</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.93939393939394</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="27489807"/>
-        <c:axId val="76562093"/>
+        <c:axId val="1375417"/>
+        <c:axId val="63927260"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="27489807"/>
+        <c:axId val="1375417"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2391,14 +2417,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="76562093"/>
+        <c:crossAx val="63927260"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76562093"/>
+        <c:axId val="63927260"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2423,7 +2449,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="27489807"/>
+        <c:crossAx val="1375417"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2463,15 +2489,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>182520</xdr:colOff>
+      <xdr:colOff>209520</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>61560</xdr:rowOff>
+      <xdr:rowOff>52560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>252360</xdr:colOff>
+      <xdr:colOff>279000</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>108720</xdr:rowOff>
+      <xdr:rowOff>108000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2479,8 +2505,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7497720" y="214920"/>
-        <a:ext cx="5759280" cy="3239280"/>
+        <a:off x="7524720" y="205920"/>
+        <a:ext cx="5758920" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2492,16 +2518,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>800280</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>14400</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>124920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>56160</xdr:colOff>
+      <xdr:colOff>82800</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>22680</xdr:rowOff>
+      <xdr:rowOff>22320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2509,8 +2535,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1612800" y="3777840"/>
-        <a:ext cx="5758560" cy="3231720"/>
+        <a:off x="1639800" y="3768840"/>
+        <a:ext cx="5758200" cy="3231360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2523,15 +2549,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>83160</xdr:colOff>
+      <xdr:colOff>110160</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>33480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>153000</xdr:colOff>
+      <xdr:colOff>179640</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>101520</xdr:rowOff>
+      <xdr:rowOff>101160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2539,8 +2565,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7398360" y="3686400"/>
-        <a:ext cx="5759280" cy="3239280"/>
+        <a:off x="7425360" y="3677400"/>
+        <a:ext cx="5758920" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2553,15 +2579,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>13680</xdr:colOff>
+      <xdr:colOff>40680</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>156240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>83160</xdr:colOff>
+      <xdr:colOff>109800</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:rowOff>161640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2569,8 +2595,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1639080" y="7305480"/>
-        <a:ext cx="5759280" cy="3239280"/>
+        <a:off x="1666080" y="7296480"/>
+        <a:ext cx="5758920" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2583,15 +2609,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>13680</xdr:colOff>
+      <xdr:colOff>40680</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>108360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>83520</xdr:colOff>
+      <xdr:colOff>110160</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:rowOff>113760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2599,8 +2625,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7328880" y="7257600"/>
-        <a:ext cx="5759280" cy="3239280"/>
+        <a:off x="7355880" y="7248600"/>
+        <a:ext cx="5758920" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2613,15 +2639,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>572400</xdr:colOff>
+      <xdr:colOff>599400</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>20520</xdr:rowOff>
+      <xdr:rowOff>11520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>641520</xdr:colOff>
+      <xdr:colOff>668160</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>76680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2629,8 +2655,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13577040" y="488160"/>
-        <a:ext cx="5758560" cy="3241800"/>
+        <a:off x="13604040" y="479160"/>
+        <a:ext cx="5758200" cy="3241440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2643,15 +2669,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>43200</xdr:colOff>
+      <xdr:colOff>70200</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>720360</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:colOff>747000</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2659,8 +2685,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1668600" y="0"/>
-        <a:ext cx="5554080" cy="3499560"/>
+        <a:off x="1695600" y="0"/>
+        <a:ext cx="5553720" cy="3499200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2681,7 +2707,7 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A52" activeCellId="0" pane="topLeft" sqref="A52"/>
+      <selection activeCell="N7" activeCellId="0" pane="topLeft" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3735,7 +3761,7 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="N2" activeCellId="0" pane="topLeft" sqref="N2"/>
+      <selection activeCell="N7" activeCellId="0" pane="topLeft" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4843,7 +4869,7 @@
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="N2" activeCellId="0" pane="topLeft" sqref="N2"/>
+      <selection activeCell="N7" activeCellId="0" pane="topLeft" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5951,8 +5977,8 @@
   </sheetPr>
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="N2" activeCellId="0" pane="topLeft" sqref="N2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="N7" activeCellId="0" pane="topLeft" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5996,7 +6022,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>11</v>
       </c>
@@ -7088,8 +7114,8 @@
   </sheetPr>
   <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B23" activeCellId="0" pane="topLeft" sqref="B23"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="R33" activeCellId="0" pane="topLeft" sqref="R33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -7126,6 +7152,7 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23"/>

</xml_diff>

<commit_message>
reorganização conclusão formatação abnt
</commit_message>
<xml_diff>
--- a/tcc_android_pattern/ckjm-1.9/metrics/analise_dados.xlsx
+++ b/tcc_android_pattern/ckjm-1.9/metrics/analise_dados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="4" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="271" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="146" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="1" state="visible" r:id="rId2"/>
@@ -412,7 +412,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="5"/>
+            <c:size val="4"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -499,11 +499,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="22213466"/>
-        <c:axId val="41284721"/>
+        <c:axId val="93281463"/>
+        <c:axId val="16024083"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="22213466"/>
+        <c:axId val="93281463"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -519,14 +519,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="41284721"/>
+        <c:crossAx val="16024083"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41284721"/>
+        <c:axId val="16024083"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -551,7 +551,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="22213466"/>
+        <c:crossAx val="93281463"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -638,7 +638,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="5"/>
+            <c:size val="4"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -725,11 +725,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="24168142"/>
-        <c:axId val="81898758"/>
+        <c:axId val="60221132"/>
+        <c:axId val="48868620"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="24168142"/>
+        <c:axId val="60221132"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -745,14 +745,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="81898758"/>
+        <c:crossAx val="48868620"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81898758"/>
+        <c:axId val="48868620"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -777,7 +777,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="24168142"/>
+        <c:crossAx val="60221132"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -864,7 +864,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="5"/>
+            <c:size val="4"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -951,11 +951,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="61533663"/>
-        <c:axId val="10940117"/>
+        <c:axId val="65022082"/>
+        <c:axId val="46262525"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="61533663"/>
+        <c:axId val="65022082"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -971,14 +971,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="10940117"/>
+        <c:crossAx val="46262525"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10940117"/>
+        <c:axId val="46262525"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1003,7 +1003,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="61533663"/>
+        <c:crossAx val="65022082"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1090,7 +1090,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="5"/>
+            <c:size val="4"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -1177,11 +1177,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="16874101"/>
-        <c:axId val="20449600"/>
+        <c:axId val="5083608"/>
+        <c:axId val="57272965"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="16874101"/>
+        <c:axId val="5083608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1197,14 +1197,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="20449600"/>
+        <c:crossAx val="57272965"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="20449600"/>
+        <c:axId val="57272965"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1229,7 +1229,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="16874101"/>
+        <c:crossAx val="5083608"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1316,7 +1316,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="5"/>
+            <c:size val="4"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -1403,11 +1403,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="68952474"/>
-        <c:axId val="80088686"/>
+        <c:axId val="46415587"/>
+        <c:axId val="25068519"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68952474"/>
+        <c:axId val="46415587"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1423,14 +1423,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="80088686"/>
+        <c:crossAx val="25068519"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80088686"/>
+        <c:axId val="25068519"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1455,7 +1455,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="68952474"/>
+        <c:crossAx val="46415587"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1524,7 +1524,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="5"/>
+            <c:size val="4"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -1592,16 +1592,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8.51612903225806</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.875</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.93939393939394</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1633,7 +1633,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="5"/>
+            <c:size val="4"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -1701,16 +1701,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.774193548387097</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.78125</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.78125</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.787878787878788</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1742,7 +1742,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="5"/>
+            <c:size val="4"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -1810,16 +1810,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1851,7 +1851,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="5"/>
+            <c:size val="4"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -1919,16 +1919,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.1612903225806</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.03125</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.09375</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.1515151515152</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1960,7 +1960,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="5"/>
+            <c:size val="4"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -2028,16 +2028,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>23.741935483871</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.21875</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.71875</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.9090909090909</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2069,7 +2069,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="5"/>
+            <c:size val="4"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -2137,27 +2137,27 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>57.4838709677419</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>56.875</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53.1875</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>48.4242424242424</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="54379820"/>
-        <c:axId val="52702933"/>
+        <c:axId val="2653443"/>
+        <c:axId val="61406965"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="54379820"/>
+        <c:axId val="2653443"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2173,14 +2173,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="52702933"/>
+        <c:crossAx val="61406965"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52702933"/>
+        <c:axId val="61406965"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2205,7 +2205,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="54379820"/>
+        <c:crossAx val="2653443"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2292,7 +2292,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="5"/>
+            <c:size val="4"/>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
@@ -2379,11 +2379,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="1375417"/>
-        <c:axId val="63927260"/>
+        <c:axId val="87169322"/>
+        <c:axId val="5119209"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1375417"/>
+        <c:axId val="87169322"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2417,14 +2417,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="63927260"/>
+        <c:crossAx val="5119209"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63927260"/>
+        <c:axId val="5119209"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2449,7 +2449,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1375417"/>
+        <c:crossAx val="87169322"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2489,15 +2489,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>209520</xdr:colOff>
+      <xdr:colOff>236520</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>52560</xdr:rowOff>
+      <xdr:rowOff>43560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>279000</xdr:colOff>
+      <xdr:colOff>305640</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>108000</xdr:rowOff>
+      <xdr:rowOff>98640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2505,8 +2505,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7524720" y="205920"/>
-        <a:ext cx="5758920" cy="3238920"/>
+        <a:off x="7551720" y="196920"/>
+        <a:ext cx="5758560" cy="3238560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2519,15 +2519,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>14400</xdr:colOff>
+      <xdr:colOff>41400</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>124920</xdr:rowOff>
+      <xdr:rowOff>115920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>82800</xdr:colOff>
+      <xdr:colOff>109440</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>22320</xdr:rowOff>
+      <xdr:rowOff>12960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2535,8 +2535,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1639800" y="3768840"/>
-        <a:ext cx="5758200" cy="3231360"/>
+        <a:off x="1666800" y="3759840"/>
+        <a:ext cx="5757840" cy="3231000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2549,15 +2549,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>110160</xdr:colOff>
+      <xdr:colOff>137160</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>33480</xdr:rowOff>
+      <xdr:rowOff>24480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>179640</xdr:colOff>
+      <xdr:colOff>206280</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>101160</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2565,8 +2565,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7425360" y="3677400"/>
-        <a:ext cx="5758920" cy="3238920"/>
+        <a:off x="7452360" y="3668400"/>
+        <a:ext cx="5758560" cy="3238560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2579,15 +2579,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>40680</xdr:colOff>
+      <xdr:colOff>67680</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>156240</xdr:rowOff>
+      <xdr:rowOff>147240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>109800</xdr:colOff>
+      <xdr:colOff>136440</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>161640</xdr:rowOff>
+      <xdr:rowOff>152280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2595,8 +2595,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1666080" y="7296480"/>
-        <a:ext cx="5758920" cy="3238920"/>
+        <a:off x="1693080" y="7287480"/>
+        <a:ext cx="5758560" cy="3238560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2609,15 +2609,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>40680</xdr:colOff>
+      <xdr:colOff>67680</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>108360</xdr:rowOff>
+      <xdr:rowOff>99360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>110160</xdr:colOff>
+      <xdr:colOff>136800</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>104400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2625,8 +2625,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7355880" y="7248600"/>
-        <a:ext cx="5758920" cy="3238920"/>
+        <a:off x="7382880" y="7239600"/>
+        <a:ext cx="5758560" cy="3238560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2639,15 +2639,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>599400</xdr:colOff>
+      <xdr:colOff>626400</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>11520</xdr:rowOff>
+      <xdr:rowOff>2520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>668160</xdr:colOff>
+      <xdr:colOff>694800</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>67320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2655,8 +2655,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13604040" y="479160"/>
-        <a:ext cx="5758200" cy="3241440"/>
+        <a:off x="13631040" y="470160"/>
+        <a:ext cx="5757840" cy="3241080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2669,15 +2669,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>70200</xdr:colOff>
+      <xdr:colOff>97200</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>747000</xdr:colOff>
+      <xdr:colOff>773640</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2685,8 +2685,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1695600" y="0"/>
-        <a:ext cx="5553720" cy="3499200"/>
+        <a:off x="1722600" y="0"/>
+        <a:ext cx="5553360" cy="3498840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2706,17 +2706,28 @@
   </sheetPr>
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="N7" activeCellId="0" pane="topLeft" sqref="N7"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="113" zoomScaleNormal="113" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="72.1581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.38265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.47959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="5.46428571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.18367346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.71428571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="4.06632653061225"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.5969387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.71428571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="4.9030612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="5.5969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3741,14 +3752,15 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="45"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="true"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="0" scale="95" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
@@ -3760,17 +3772,29 @@
   </sheetPr>
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="N7" activeCellId="0" pane="topLeft" sqref="N7"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="77.25"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.83163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.04591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.87755102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.70408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.26020408163265"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="4.31122448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.87755102040816"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.26020408163265"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="5.18367346938776"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="5.70408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4357,7 +4381,7 @@
         <v>-0.608870967741936</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.95" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
         <v>26</v>
       </c>
@@ -4851,12 +4875,12 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="true"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="0" scale="90" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
@@ -4868,8 +4892,8 @@
   </sheetPr>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="N7" activeCellId="0" pane="topLeft" sqref="N7"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5977,8 +6001,8 @@
   </sheetPr>
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="N7" activeCellId="0" pane="topLeft" sqref="N7"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -6242,7 +6266,7 @@
         <v>24.9090909090909</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
         <v>18</v>
       </c>
@@ -7114,8 +7138,8 @@
   </sheetPr>
   <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="R33" activeCellId="0" pane="topLeft" sqref="R33"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>